<commit_message>
FX module - front panel wip
</commit_message>
<xml_diff>
--- a/modules/FX/panel/positions.xlsx
+++ b/modules/FX/panel/positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB258E8-1BFB-4A6A-BC4C-35502690868E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A0A16-DA6B-4515-A24E-9F8E66927D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1845" windowWidth="19380" windowHeight="11835" xr2:uid="{B2D59E76-B88C-43E0-9F83-1CEB42A2BB3E}"/>
+    <workbookView xWindow="6060" yWindow="2760" windowWidth="19380" windowHeight="11835" xr2:uid="{B2D59E76-B88C-43E0-9F83-1CEB42A2BB3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>PCB</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>top extra</t>
+  </si>
+  <si>
+    <t>panel SVG</t>
+  </si>
+  <si>
+    <t>diameter</t>
   </si>
 </sst>
 </file>
@@ -432,23 +438,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D06F73C-F6DB-42E2-BEE4-47F1680D293F}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -462,10 +471,22 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -481,11 +502,17 @@
       <c r="E3">
         <v>50</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>10.16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>50</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -500,11 +527,25 @@
         <v>80.153000000000006</v>
       </c>
       <c r="E4">
-        <f>C4-C$3+E$3+$F$3</f>
+        <f>C4-C$3+E$3+$G$3</f>
         <v>65.359380000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f>D4-D$3+H$3-$J4/2</f>
+        <v>67.653000000000006</v>
+      </c>
+      <c r="I4">
+        <f>E4-E$3+I$3-$J4/2</f>
+        <v>62.859380000000002</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -520,11 +561,25 @@
         <v>70.805800000000005</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E12" si="1">C5-C$3+E$3+$F$3</f>
+        <f t="shared" ref="E5:E12" si="1">C5-C$3+E$3+$G$3</f>
         <v>86.87</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>9.5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H12" si="2">D5-D$3+H$3-$J5/2</f>
+        <v>56.055800000000005</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I12" si="3">E5-E$3+I$3-$J5/2</f>
+        <v>82.12</v>
+      </c>
+      <c r="J5">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -542,8 +597,22 @@
         <f t="shared" si="1"/>
         <v>86.87</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>7.3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>76.000000000000014</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>83.37</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -561,8 +630,22 @@
         <f t="shared" si="1"/>
         <v>110.46</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>7.3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>57.305800000000005</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>106.96</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -580,8 +663,22 @@
         <f t="shared" si="1"/>
         <v>110.46</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>7.3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>76.000000000000014</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>106.96</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -599,8 +696,22 @@
         <f t="shared" si="1"/>
         <v>136.447</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>7.3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>66.653000000000006</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>132.947</v>
+      </c>
+      <c r="J9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -618,8 +729,22 @@
         <f t="shared" si="1"/>
         <v>162.0556</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>6.3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>52.67</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>159.0556</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -637,8 +762,22 @@
         <f t="shared" si="1"/>
         <v>162.0556</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>6.3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>71.912500000000009</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>159.0556</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -655,6 +794,20 @@
       <c r="E12">
         <f t="shared" si="1"/>
         <v>162.0556</v>
+      </c>
+      <c r="F12">
+        <v>6.3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>81.437500000000014</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>159.0556</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FX module - front panel adjustments
</commit_message>
<xml_diff>
--- a/modules/FX/panel/positions.xlsx
+++ b/modules/FX/panel/positions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2A0A16-DA6B-4515-A24E-9F8E66927D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC7D9AC-BEEC-4F00-80CA-3BAA5869B2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="2760" windowWidth="19380" windowHeight="11835" xr2:uid="{B2D59E76-B88C-43E0-9F83-1CEB42A2BB3E}"/>
+    <workbookView xWindow="7560" yWindow="1605" windowWidth="19380" windowHeight="11835" xr2:uid="{B2D59E76-B88C-43E0-9F83-1CEB42A2BB3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
         <v>111.1358</v>
       </c>
       <c r="C5">
-        <v>63.54</v>
+        <v>61.142380000000003</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D12" si="0">B5-B$3+D$3</f>
@@ -562,7 +562,7 @@
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E12" si="1">C5-C$3+E$3+$G$3</f>
-        <v>86.87</v>
+        <v>84.472380000000001</v>
       </c>
       <c r="F5">
         <v>9.5</v>
@@ -573,7 +573,7 @@
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I12" si="3">E5-E$3+I$3-$J5/2</f>
-        <v>82.12</v>
+        <v>79.722380000000001</v>
       </c>
       <c r="J5">
         <v>9.5</v>
@@ -587,7 +587,7 @@
         <v>129.83000000000001</v>
       </c>
       <c r="C6">
-        <v>63.54</v>
+        <v>61.143000000000001</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -595,7 +595,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>86.87</v>
+        <v>84.472999999999999</v>
       </c>
       <c r="F6">
         <v>7.3</v>
@@ -606,7 +606,7 @@
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>83.37</v>
+        <v>80.972999999999999</v>
       </c>
       <c r="J6">
         <v>7</v>

</xml_diff>